<commit_message>
Added Translation to Dict for MeetOpt and Event lists
</commit_message>
<xml_diff>
--- a/FieldNamesRelationToMeetopt.xlsx
+++ b/FieldNamesRelationToMeetopt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdb025\Documents\GitHub\collegeswimming.com-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7CB80C-B0FF-4DC1-AF08-B60F5FD22BE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336D0991-3C54-4F33-ACBD-C065BF1F13D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{C169DD18-BCB7-4808-AF36-AFBAE24A835A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="93">
   <si>
     <t>F1200Y</t>
   </si>
@@ -229,6 +229,81 @@
   </si>
   <si>
     <t>200BR</t>
+  </si>
+  <si>
+    <t>indiv</t>
+  </si>
+  <si>
+    <t>MeetOpt Dec Vars</t>
+  </si>
+  <si>
+    <t>xvar</t>
+  </si>
+  <si>
+    <t>xvar, yvar, zvar</t>
+  </si>
+  <si>
+    <t>relaynoMR</t>
+  </si>
+  <si>
+    <t>xvarstart</t>
+  </si>
+  <si>
+    <t>yvarstart</t>
+  </si>
+  <si>
+    <t>yvar</t>
+  </si>
+  <si>
+    <t>zvarstart</t>
+  </si>
+  <si>
+    <t>zvar</t>
+  </si>
+  <si>
+    <t>xMRvar</t>
+  </si>
+  <si>
+    <t>yMRvar</t>
+  </si>
+  <si>
+    <t>zMRvar</t>
+  </si>
+  <si>
+    <t>stroke</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>event_noMR</t>
+  </si>
+  <si>
+    <t>Array2</t>
+  </si>
+  <si>
+    <t>Array1</t>
+  </si>
+  <si>
+    <t>event11 is the list of all scored events in a meet!</t>
+  </si>
+  <si>
+    <t>playperfMR[athlete][stroke]</t>
+  </si>
+  <si>
+    <t>playperfstart[athlete][relaynoMR]</t>
+  </si>
+  <si>
+    <t>playperf[athlete][event]</t>
+  </si>
+  <si>
+    <t>player performance</t>
+  </si>
+  <si>
+    <t>playperf[ath][indiv]</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -272,9 +347,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24326742-2BED-4210-80BB-39CD9EA80C07}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,9 +678,11 @@
     <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -629,8 +707,20 @@
       <c r="H1" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -655,8 +745,20 @@
       <c r="H2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -681,8 +783,20 @@
       <c r="H3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -707,8 +821,20 @@
       <c r="H4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
+      </c>
+      <c r="M4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -733,8 +859,20 @@
       <c r="H5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -759,8 +897,20 @@
       <c r="H6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -785,8 +935,20 @@
       <c r="H7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -811,8 +973,20 @@
       <c r="H8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -837,8 +1011,20 @@
       <c r="H9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" t="s">
+        <v>83</v>
+      </c>
+      <c r="M9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -863,8 +1049,20 @@
       <c r="H10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" t="s">
+        <v>83</v>
+      </c>
+      <c r="M10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -889,8 +1087,20 @@
       <c r="H11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" t="s">
+        <v>83</v>
+      </c>
+      <c r="M11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -915,8 +1125,20 @@
       <c r="H12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -941,8 +1163,20 @@
       <c r="H13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" t="s">
+        <v>83</v>
+      </c>
+      <c r="M13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -964,8 +1198,20 @@
       <c r="G14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -987,8 +1233,17 @@
       <c r="G15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1010,8 +1265,17 @@
       <c r="G16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1033,8 +1297,17 @@
       <c r="G17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1056,8 +1329,17 @@
       <c r="G18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I18" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1079,8 +1361,17 @@
       <c r="G19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1102,8 +1393,17 @@
       <c r="G20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" t="s">
+        <v>79</v>
+      </c>
+      <c r="M20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1125,8 +1425,17 @@
       <c r="G21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" t="s">
+        <v>79</v>
+      </c>
+      <c r="M21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1148,8 +1457,17 @@
       <c r="G22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I22" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" t="s">
+        <v>80</v>
+      </c>
+      <c r="M22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1171,8 +1489,17 @@
       <c r="G23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1194,8 +1521,17 @@
       <c r="G24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" t="s">
+        <v>80</v>
+      </c>
+      <c r="M24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1217,8 +1553,17 @@
       <c r="G25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I25" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" t="s">
+        <v>80</v>
+      </c>
+      <c r="M25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1240,8 +1585,17 @@
       <c r="G26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I26" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" t="s">
+        <v>82</v>
+      </c>
+      <c r="M26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1263,8 +1617,17 @@
       <c r="G27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I27" t="s">
+        <v>82</v>
+      </c>
+      <c r="J27" t="s">
+        <v>82</v>
+      </c>
+      <c r="M27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1286,8 +1649,17 @@
       <c r="G28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I28" t="s">
+        <v>82</v>
+      </c>
+      <c r="J28" t="s">
+        <v>82</v>
+      </c>
+      <c r="M28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1309,8 +1681,17 @@
       <c r="G29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I29" t="s">
+        <v>82</v>
+      </c>
+      <c r="J29" t="s">
+        <v>82</v>
+      </c>
+      <c r="M29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1332,8 +1713,14 @@
       <c r="G30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J30" t="s">
+        <v>73</v>
+      </c>
+      <c r="M30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1355,8 +1742,17 @@
       <c r="G31" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I31" t="s">
+        <v>72</v>
+      </c>
+      <c r="J31" t="s">
+        <v>70</v>
+      </c>
+      <c r="M31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1378,8 +1774,14 @@
       <c r="G32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J32" t="s">
+        <v>74</v>
+      </c>
+      <c r="M32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1401,8 +1803,17 @@
       <c r="G33" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I33" t="s">
+        <v>72</v>
+      </c>
+      <c r="J33" t="s">
+        <v>75</v>
+      </c>
+      <c r="M33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1424,8 +1835,14 @@
       <c r="G34" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J34" t="s">
+        <v>76</v>
+      </c>
+      <c r="M34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1447,8 +1864,17 @@
       <c r="G35" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J35" t="s">
+        <v>77</v>
+      </c>
+      <c r="M35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1470,8 +1896,14 @@
       <c r="G36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J36" t="s">
+        <v>53</v>
+      </c>
+      <c r="M36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1492,6 +1924,20 @@
       </c>
       <c r="G37" t="s">
         <v>48</v>
+      </c>
+      <c r="I37" t="s">
+        <v>72</v>
+      </c>
+      <c r="J37" t="s">
+        <v>53</v>
+      </c>
+      <c r="M37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>